<commit_message>
Changed the environment Modified test runner Modified testcase names added new tc and relavent methods
</commit_message>
<xml_diff>
--- a/TestRunner.xlsx
+++ b/TestRunner.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Messages121Test</t>
   </si>
   <si>
-    <t xml:space="preserve">safari</t>
+    <t xml:space="preserve">chrome</t>
   </si>
   <si>
     <t xml:space="preserve">QA</t>
@@ -297,8 +297,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added 2 pending TC's and updated elements w.r.t dev environment
</commit_message>
<xml_diff>
--- a/TestRunner.xlsx
+++ b/TestRunner.xlsx
@@ -297,8 +297,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>